<commit_message>
attempting to fix post times
</commit_message>
<xml_diff>
--- a/Client/src/main/java/TestingResults.xlsx
+++ b/Client/src/main/java/TestingResults.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Northeastern\CS6650\CS6650-Assignment1\Client\src\main\java\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
   <si>
     <t>Test Type</t>
   </si>
@@ -75,7 +75,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,14 +458,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="38.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="33.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -933,6 +934,578 @@
       </c>
       <c r="H18">
         <v>347.97399999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>23.25581395348837</v>
+      </c>
+      <c r="H19" t="n">
+        <v>8.795</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6.515000000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>38.46153846153846</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5.2090000000000005</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5.163</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>322.5806451612903</v>
+      </c>
+      <c r="H23" t="n">
+        <v>6.596</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>400.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5.331</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>384.6153846153846</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5.609</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>136.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>735.2941176470588</v>
+      </c>
+      <c r="H26" t="n">
+        <v>47.656</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>357.1428571428571</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5.862</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1176.4705882352941</v>
+      </c>
+      <c r="H28" t="n">
+        <v>35.322</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>370.3703703703704</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5.982</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>200000.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>200000.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>176.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>568.1818181818182</v>
+      </c>
+      <c r="H30" t="n">
+        <v>373.163</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>370.3703703703704</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5.843</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1204.8192771084337</v>
+      </c>
+      <c r="H32" t="n">
+        <v>34.633</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>370.3703703703704</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5.613</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>357.1428571428571</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5.912</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>862.0689655172413</v>
+      </c>
+      <c r="H35" t="n">
+        <v>43.914</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>384.6153846153846</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5.632</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>694.4444444444443</v>
+      </c>
+      <c r="H37" t="n">
+        <v>51.174</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>370.3703703703704</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5.672</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>384.6153846153846</v>
+      </c>
+      <c r="H39" t="n">
+        <v>5.589</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>20000.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1234.567901234568</v>
+      </c>
+      <c r="H40" t="n">
+        <v>33.965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>